<commit_message>
some changes for env and results
</commit_message>
<xml_diff>
--- a/automated_results/logfc-genes-overall.xlsx
+++ b/automated_results/logfc-genes-overall.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Gene.ID</t>
   </si>
@@ -28,6 +28,45 @@
   </si>
   <si>
     <t>GSE89632</t>
+  </si>
+  <si>
+    <t>FOS</t>
+  </si>
+  <si>
+    <t>IGFBP1</t>
+  </si>
+  <si>
+    <t>IGFBP2</t>
+  </si>
+  <si>
+    <t>THBS1</t>
+  </si>
+  <si>
+    <t>IRS2</t>
+  </si>
+  <si>
+    <t>SOCS2</t>
+  </si>
+  <si>
+    <t>UBD</t>
+  </si>
+  <si>
+    <t>GADD45G</t>
+  </si>
+  <si>
+    <t>DNMT3L</t>
+  </si>
+  <si>
+    <t>GOLM1</t>
+  </si>
+  <si>
+    <t>ANGPTL8</t>
+  </si>
+  <si>
+    <t>EFHD1</t>
+  </si>
+  <si>
+    <t>CRISPLD2</t>
   </si>
   <si>
     <t>logFC</t>
@@ -43,15 +82,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
+      <color theme="1"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
+      <i/>
+      <color theme="1"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +124,12 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -83,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -95,6 +155,10 @@
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,6 +704,9 @@
       <c r="D2" s="3">
         <v>2.886247</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1">
@@ -654,6 +721,9 @@
       <c r="D3" s="3">
         <v>2.252961</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1">
@@ -668,6 +738,9 @@
       <c r="D4" s="3">
         <v>1.5424469999999999</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1">
@@ -682,6 +755,9 @@
       <c r="D5" s="3">
         <v>1.807104</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1">
@@ -696,6 +772,9 @@
       <c r="D6" s="3">
         <v>1.1009249999999999</v>
       </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1">
@@ -710,6 +789,9 @@
       <c r="D7" s="3">
         <v>2.1203759999999998</v>
       </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1">
@@ -724,6 +806,9 @@
       <c r="D8" s="4">
         <v>-1.1543779999999999</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1">
@@ -738,6 +823,9 @@
       <c r="D9" s="3">
         <v>2.7345190000000001</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="1">
@@ -752,6 +840,9 @@
       <c r="D10" s="4">
         <v>-1.0596410000000001</v>
       </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="1">
@@ -766,6 +857,9 @@
       <c r="D11" s="4">
         <v>-1.0929040000000001</v>
       </c>
+      <c r="E11" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="1">
@@ -780,6 +874,9 @@
       <c r="D12" s="4">
         <v>-1.6701269999999999</v>
       </c>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="1">
@@ -794,6 +891,9 @@
       <c r="D13" s="3">
         <v>1.0647070000000001</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="1">
@@ -808,11 +908,16 @@
       <c r="D14" s="3">
         <v>1.3672850000000001</v>
       </c>
-    </row>
+      <c r="E14" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25"/>
+    <row r="16" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -824,7 +929,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="3" max="4" width="11.76171875"/>
   </cols>
@@ -834,25 +939,14 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -867,7 +961,6 @@
       <c r="D2">
         <v>0.041125099999999998</v>
       </c>
-      <c r="E2"/>
     </row>
     <row r="3">
       <c r="A3">
@@ -952,7 +1045,6 @@
       <c r="D8">
         <v>0.00097542549999999999</v>
       </c>
-      <c r="E8"/>
     </row>
     <row r="9">
       <c r="A9">
@@ -981,7 +1073,6 @@
       <c r="D10">
         <v>0.015109030000000001</v>
       </c>
-      <c r="E10"/>
     </row>
     <row r="11">
       <c r="A11">
@@ -1024,7 +1115,6 @@
       <c r="D13">
         <v>5.3655510000000002e-05</v>
       </c>
-      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14">
@@ -1049,7 +1139,7 @@
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1061,7 +1151,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="2" max="2" width="9.28125"/>
     <col bestFit="1" min="3" max="3" width="11.76171875"/>
@@ -1073,22 +1163,14 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="N1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -1103,7 +1185,6 @@
       <c r="D2">
         <v>0.000202</v>
       </c>
-      <c r="F2"/>
     </row>
     <row r="3">
       <c r="A3">
@@ -1118,7 +1199,6 @@
       <c r="D3">
         <v>0.00061799999999999995</v>
       </c>
-      <c r="F3"/>
     </row>
     <row r="4">
       <c r="A4">
@@ -1133,7 +1213,6 @@
       <c r="D4">
         <v>0.0065059999999999996</v>
       </c>
-      <c r="F4"/>
     </row>
     <row r="5">
       <c r="A5">
@@ -1148,7 +1227,6 @@
       <c r="D5">
         <v>0.013028</v>
       </c>
-      <c r="F5"/>
     </row>
     <row r="6">
       <c r="A6">
@@ -1163,8 +1241,6 @@
       <c r="D6">
         <v>0.0032290000000000001</v>
       </c>
-      <c r="E6"/>
-      <c r="F6"/>
     </row>
     <row r="7">
       <c r="A7">
@@ -1179,7 +1255,6 @@
       <c r="D7">
         <v>0.013058</v>
       </c>
-      <c r="F7"/>
     </row>
     <row r="8">
       <c r="A8">
@@ -1194,7 +1269,6 @@
       <c r="D8">
         <v>0.032842999999999997</v>
       </c>
-      <c r="F8"/>
     </row>
     <row r="9">
       <c r="A9">
@@ -1209,7 +1283,6 @@
       <c r="D9">
         <v>0.019467999999999999</v>
       </c>
-      <c r="F9"/>
     </row>
     <row r="10">
       <c r="A10">
@@ -1224,7 +1297,6 @@
       <c r="D10">
         <v>0.012399</v>
       </c>
-      <c r="F10"/>
     </row>
     <row r="11">
       <c r="A11">
@@ -1239,8 +1311,6 @@
       <c r="D11">
         <v>0.044967</v>
       </c>
-      <c r="E11"/>
-      <c r="F11"/>
     </row>
     <row r="12">
       <c r="A12">
@@ -1255,8 +1325,6 @@
       <c r="D12">
         <v>0.022391999999999999</v>
       </c>
-      <c r="E12"/>
-      <c r="F12"/>
     </row>
     <row r="13">
       <c r="A13">
@@ -1271,7 +1339,6 @@
       <c r="D13">
         <v>0.044218</v>
       </c>
-      <c r="F13"/>
     </row>
     <row r="14">
       <c r="A14">
@@ -1286,8 +1353,6 @@
       <c r="D14">
         <v>0.015661000000000001</v>
       </c>
-      <c r="E14"/>
-      <c r="F14"/>
     </row>
     <row r="15"/>
   </sheetData>
@@ -1296,7 +1361,7 @@
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1308,7 +1373,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="2" max="2" width="9.28125"/>
     <col bestFit="1" min="3" max="3" width="11.3828125"/>
@@ -1320,25 +1385,14 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -1409,7 +1463,6 @@
       <c r="D6">
         <v>0.00038671069999999998</v>
       </c>
-      <c r="E6"/>
     </row>
     <row r="7">
       <c r="A7">
@@ -1466,7 +1519,6 @@
       <c r="D10">
         <v>0.0001749105</v>
       </c>
-      <c r="E10"/>
     </row>
     <row r="11">
       <c r="A11">
@@ -1481,7 +1533,6 @@
       <c r="D11">
         <v>0.00010097449999999999</v>
       </c>
-      <c r="E11"/>
     </row>
     <row r="12">
       <c r="A12">
@@ -1496,7 +1547,6 @@
       <c r="D12">
         <v>2.9245730000000001e-10</v>
       </c>
-      <c r="E12"/>
     </row>
     <row r="13">
       <c r="A13">
@@ -1535,7 +1585,7 @@
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>